<commit_message>
upgrade targets com flag acordo
</commit_message>
<xml_diff>
--- a/targets/gabarito_ever_over.xlsx
+++ b/targets/gabarito_ever_over.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JM\Documents\0_CienciaDados\2_Mentoria_Risco_Credito\ENCONTRO_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JM\Documents\0_CienciaDados\1_Frameworks\creditlab\targets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3947F138-E1D8-454D-951A-72A6FA1AE155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8296E2D6-59EA-4CFD-B641-8A65FA811678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B5986926-A03F-4519-8581-817F09413AF3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>safra_ref</t>
   </si>
@@ -52,6 +52,18 @@
   </si>
   <si>
     <t>gabarito_over90m12</t>
+  </si>
+  <si>
+    <t>flag_acordo</t>
+  </si>
+  <si>
+    <t>gabarito_bad90</t>
+  </si>
+  <si>
+    <t>gabarito_target_ever90m12</t>
+  </si>
+  <si>
+    <t>gabarito_target_over90m12</t>
   </si>
 </sst>
 </file>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A02A1F07-3206-4D4B-B8DB-214128CB1343}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,9 +431,12 @@
     <col min="3" max="3" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="25.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +455,20 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>202001</v>
       </c>
@@ -456,15 +483,30 @@
         <v>0</v>
       </c>
       <c r="E2" s="1">
-        <f>IF(C14&gt;=90,1,0)</f>
+        <f t="shared" ref="E2:E37" si="0">IF(C14&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="F2" s="1">
         <f>IF(SUM(D3:D14)&gt;=1,1,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <f>IF(OR(C2&gt;=90,G2=1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
+        <f>IF(SUM(H3:H14)&gt;=1,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <f>IF(H14&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>202002</v>
       </c>
@@ -475,19 +517,34 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D37" si="0">IF(C3&gt;=90,1,0)</f>
+        <f>IF(C3&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E3" s="1">
-        <f>IF(C15&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F37" si="1">IF(SUM(D4:D15)&gt;=1,1,0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <f>IF(OR(C3&gt;=90,G3=1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I37" si="2">IF(SUM(H4:H15)&gt;=1,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J3" s="1">
+        <f t="shared" ref="J3:J37" si="3">IF(H15&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>202003</v>
       </c>
@@ -498,19 +555,34 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C4&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <f>IF(C16&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <f t="shared" ref="H4:H37" si="4">IF(OR(C4&gt;=90,G4=1),1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>202004</v>
       </c>
@@ -521,19 +593,34 @@
         <v>15</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C5&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E5" s="1">
-        <f>IF(C17&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>202005</v>
       </c>
@@ -544,19 +631,34 @@
         <v>45</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C6&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <f>IF(C18&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>202006</v>
       </c>
@@ -567,19 +669,34 @@
         <v>75</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C7&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E7" s="1">
-        <f>IF(C19&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>202007</v>
       </c>
@@ -590,19 +707,34 @@
         <v>0</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C8&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <f>IF(C20&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>202008</v>
       </c>
@@ -613,19 +745,34 @@
         <v>0</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C9&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E9" s="1">
-        <f>IF(C21&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>202009</v>
       </c>
@@ -636,19 +783,34 @@
         <v>0</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C10&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <f>IF(C22&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>202010</v>
       </c>
@@ -659,19 +821,34 @@
         <v>0</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C11&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E11" s="1">
-        <f>IF(C23&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>202011</v>
       </c>
@@ -682,19 +859,34 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C12&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <f>IF(C24&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>202012</v>
       </c>
@@ -705,19 +897,34 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C13&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E13" s="1">
-        <f>IF(C25&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>202101</v>
       </c>
@@ -728,19 +935,34 @@
         <v>12</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C14&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <f>IF(C26&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>202102</v>
       </c>
@@ -751,19 +973,34 @@
         <v>42</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C15&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E15" s="1">
-        <f>IF(C27&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>202103</v>
       </c>
@@ -774,19 +1011,34 @@
         <v>72</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C16&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E16" s="1">
-        <f>IF(C28&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>202104</v>
       </c>
@@ -797,19 +1049,34 @@
         <v>102</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C17&gt;=90,1,0)</f>
         <v>1</v>
       </c>
       <c r="E17" s="1">
-        <f>IF(C29&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>202105</v>
       </c>
@@ -820,19 +1087,34 @@
         <v>0</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C18&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f>IF(C30&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>202106</v>
       </c>
@@ -843,19 +1125,34 @@
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C19&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E19" s="1">
-        <f>IF(C31&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>202107</v>
       </c>
@@ -866,19 +1163,34 @@
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C20&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E20" s="1">
-        <f>IF(C32&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>202108</v>
       </c>
@@ -889,19 +1201,34 @@
         <v>0</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C21&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <f>IF(C33&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>202109</v>
       </c>
@@ -912,19 +1239,34 @@
         <v>0</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C22&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E22" s="1">
-        <f>IF(C34&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>202110</v>
       </c>
@@ -935,19 +1277,34 @@
         <v>0</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C23&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E23" s="1">
-        <f>IF(C35&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>202111</v>
       </c>
@@ -958,19 +1315,34 @@
         <v>10</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C24&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <f>IF(C36&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>202112</v>
       </c>
@@ -981,19 +1353,34 @@
         <v>25</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C25&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E25" s="1">
-        <f>IF(C37&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>202201</v>
       </c>
@@ -1004,19 +1391,34 @@
         <v>0</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C26&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E26" s="1">
-        <f>IF(C38&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J26" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>202202</v>
       </c>
@@ -1027,19 +1429,34 @@
         <v>0</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C27&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <f>IF(C39&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>202203</v>
       </c>
@@ -1050,19 +1467,34 @@
         <v>0</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C28&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <f>IF(C40&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>202204</v>
       </c>
@@ -1073,19 +1505,34 @@
         <v>0</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C29&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E29" s="1">
-        <f>IF(C41&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J29" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>202205</v>
       </c>
@@ -1096,19 +1543,34 @@
         <v>0</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C30&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <f>IF(C42&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J30" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>202206</v>
       </c>
@@ -1119,19 +1581,34 @@
         <v>0</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C31&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E31" s="1">
-        <f>IF(C43&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>202207</v>
       </c>
@@ -1142,19 +1619,34 @@
         <v>0</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C32&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E32" s="1">
-        <f>IF(C44&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J32" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>202208</v>
       </c>
@@ -1165,19 +1657,34 @@
         <v>5</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C33&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <f>IF(C45&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F33" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J33" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>202209</v>
       </c>
@@ -1188,19 +1695,34 @@
         <v>15</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C34&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <f>IF(C46&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F34" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>202210</v>
       </c>
@@ -1211,19 +1733,34 @@
         <v>30</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C35&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E35" s="1">
-        <f>IF(C47&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F35" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J35" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>202211</v>
       </c>
@@ -1234,19 +1771,34 @@
         <v>60</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C36&gt;=90,1,0)</f>
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <f>IF(C48&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F36" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36" s="1">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J36" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>202212</v>
       </c>
@@ -1257,15 +1809,30 @@
         <v>90</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
+        <f>IF(C37&gt;=90,1,0)</f>
         <v>1</v>
       </c>
       <c r="E37" s="1">
-        <f>IF(C49&gt;=90,1,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F37" s="1">
         <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="1">
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>